<commit_message>
add speedup factor to excel
</commit_message>
<xml_diff>
--- a/Info_praktikum/BS-Praktikum/Aufgabe2/Threads.xlsx
+++ b/Info_praktikum/BS-Praktikum/Aufgabe2/Threads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\daten\Informatik\repos\fah5625\Info_praktikum\BS-Praktikum\Aufgabe2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09326817-22CF-4E90-9CD1-064B1B52F8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD44980-8158-4B34-A839-9E5031C4F49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Threads:</t>
   </si>
@@ -53,7 +53,19 @@
     <t>Atomic (s)</t>
   </si>
   <si>
-    <t>Speedup Faktor</t>
+    <t>Speedup Mutex</t>
+  </si>
+  <si>
+    <t>Speedup Sem</t>
+  </si>
+  <si>
+    <t>Speedup Atomic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speedup </t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -98,7 +110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -189,19 +201,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -230,24 +229,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -265,34 +253,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -324,19 +284,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -399,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,52 +363,70 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2037,20 +2002,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A11:Q17"/>
+  <dimension ref="A11:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="11" spans="1:17" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:17" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="15">
         <v>1</v>
       </c>
       <c r="C12" s="1">
@@ -2100,7 +2065,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="3">
@@ -2148,15 +2113,15 @@
       <c r="P13" s="4">
         <v>16.723106999999999</v>
       </c>
-      <c r="Q13" s="14">
+      <c r="Q13" s="10">
         <v>16.685355999999999</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>127.90370900000001</v>
       </c>
       <c r="C14" s="5">
@@ -2201,15 +2166,15 @@
       <c r="P14" s="5">
         <v>16.706968</v>
       </c>
-      <c r="Q14" s="15">
+      <c r="Q14" s="11">
         <v>16.486902000000001</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>127.17151699999999</v>
       </c>
       <c r="C15" s="5">
@@ -2254,129 +2219,333 @@
       <c r="P15" s="5">
         <v>16.933311</v>
       </c>
-      <c r="Q15" s="15">
+      <c r="Q15" s="11">
         <v>16.846879999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:17" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="12">
         <v>127.404866</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="23">
         <v>67.396302000000006</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="23">
         <v>44.899217999999998</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="23">
         <v>35.592323999999998</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="23">
         <v>29.944723</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="23">
         <v>26.213974</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="23">
         <v>23.221820000000001</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="23">
         <v>21.178865999999999</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="23">
         <v>19.29363</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="23">
         <v>18.520502</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="23">
         <v>18.025866000000001</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="23">
         <v>17.548333</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="23">
         <v>17.111708</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="23">
         <v>16.822392000000001</v>
       </c>
-      <c r="P16" s="6">
+      <c r="P16" s="23">
         <v>16.547854000000001</v>
       </c>
-      <c r="Q16" s="16">
+      <c r="Q16" s="24">
         <v>16.45196</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="18">
+    <row r="17" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="22">
         <f>$B$13/C13</f>
         <v>1.9060503913348505</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="22">
         <f t="shared" ref="D17:Q17" si="0">$B$13/D13</f>
         <v>2.8128231649997084</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="22">
         <f t="shared" si="0"/>
         <v>3.5524048113124032</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="22">
         <f t="shared" si="0"/>
         <v>4.2061900572826199</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="22">
         <f t="shared" si="0"/>
         <v>4.9058340093452566</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="22">
         <f t="shared" si="0"/>
         <v>5.4268897028989027</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="22">
         <f t="shared" si="0"/>
         <v>5.9801935485210116</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="22">
         <f t="shared" si="0"/>
         <v>6.3843153191069968</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="22">
         <f t="shared" si="0"/>
         <v>6.6584225189479271</v>
       </c>
-      <c r="L17" s="18">
+      <c r="L17" s="22">
         <f t="shared" si="0"/>
         <v>6.9466453779865898</v>
       </c>
-      <c r="M17" s="18">
+      <c r="M17" s="22">
         <f t="shared" si="0"/>
         <v>7.1523762839503897</v>
       </c>
-      <c r="N17" s="18">
+      <c r="N17" s="22">
         <f t="shared" si="0"/>
         <v>7.3367713137364454</v>
       </c>
-      <c r="O17" s="18">
+      <c r="O17" s="22">
         <f t="shared" si="0"/>
         <v>7.515602951079015</v>
       </c>
-      <c r="P17" s="18">
+      <c r="P17" s="22">
         <f t="shared" si="0"/>
         <v>7.5804152302559569</v>
       </c>
-      <c r="Q17" s="19">
+      <c r="Q17" s="25">
         <f t="shared" si="0"/>
         <v>7.5975660932856339</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="5">
+        <f>$B$14/C14</f>
+        <v>1.9060864463375107</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" ref="D18:Q18" si="1">$B$14/D14</f>
+        <v>2.8182596290572781</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>3.5742636392069085</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1911087894112136</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="1"/>
+        <v>4.9745449531807386</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="1"/>
+        <v>5.5955054651060134</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" si="1"/>
+        <v>6.1008621665837186</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="1"/>
+        <v>6.5446806823156249</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="1"/>
+        <v>6.8249002814402679</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" si="1"/>
+        <v>7.0888157969485057</v>
+      </c>
+      <c r="M18" s="5">
+        <f t="shared" si="1"/>
+        <v>7.3404610261230765</v>
+      </c>
+      <c r="N18" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5228010428570196</v>
+      </c>
+      <c r="O18" s="5">
+        <f t="shared" si="1"/>
+        <v>7.643157537640862</v>
+      </c>
+      <c r="P18" s="5">
+        <f t="shared" si="1"/>
+        <v>7.6557104197482158</v>
+      </c>
+      <c r="Q18" s="11">
+        <f t="shared" si="1"/>
+        <v>7.7578983001172688</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="17">
+        <f>$B$15/C15</f>
+        <v>1.904187680560268</v>
+      </c>
+      <c r="D19" s="17">
+        <f t="shared" ref="D19:Q19" si="2">$B$15/D15</f>
+        <v>2.8283106897704222</v>
+      </c>
+      <c r="E19" s="17">
+        <f t="shared" si="2"/>
+        <v>3.5707396301463197</v>
+      </c>
+      <c r="F19" s="17">
+        <f t="shared" si="2"/>
+        <v>4.2556765017678897</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="2"/>
+        <v>4.9974936985841856</v>
+      </c>
+      <c r="H19" s="17">
+        <f t="shared" si="2"/>
+        <v>5.5158719632054041</v>
+      </c>
+      <c r="I19" s="17">
+        <f t="shared" si="2"/>
+        <v>6.1162179609973961</v>
+      </c>
+      <c r="J19" s="17">
+        <f t="shared" si="2"/>
+        <v>6.5072023027556289</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" si="2"/>
+        <v>6.8317445253490314</v>
+      </c>
+      <c r="L19" s="17">
+        <f t="shared" si="2"/>
+        <v>7.0979961083999594</v>
+      </c>
+      <c r="M19" s="17">
+        <f t="shared" si="2"/>
+        <v>7.1538029600538815</v>
+      </c>
+      <c r="N19" s="17">
+        <f t="shared" si="2"/>
+        <v>7.3564869881916977</v>
+      </c>
+      <c r="O19" s="17">
+        <f t="shared" si="2"/>
+        <v>7.4116099850685551</v>
+      </c>
+      <c r="P19" s="17">
+        <f t="shared" si="2"/>
+        <v>7.5101388617973175</v>
+      </c>
+      <c r="Q19" s="27">
+        <f t="shared" si="2"/>
+        <v>7.5486687742774929</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="13">
+        <f>$B$16/C16</f>
+        <v>1.8903836296537455</v>
+      </c>
+      <c r="D20" s="13">
+        <f t="shared" ref="D20:Q20" si="3">$B$16/D16</f>
+        <v>2.8375742757925093</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="3"/>
+        <v>3.5795601883147614</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" si="3"/>
+        <v>4.2546683767954709</v>
+      </c>
+      <c r="G20" s="13">
+        <f t="shared" si="3"/>
+        <v>4.8601889206115789</v>
+      </c>
+      <c r="H20" s="13">
+        <f t="shared" si="3"/>
+        <v>5.4864289706836065</v>
+      </c>
+      <c r="I20" s="13">
+        <f t="shared" si="3"/>
+        <v>6.0156604229895976</v>
+      </c>
+      <c r="J20" s="13">
+        <f t="shared" si="3"/>
+        <v>6.6034678803314879</v>
+      </c>
+      <c r="K20" s="13">
+        <f t="shared" si="3"/>
+        <v>6.8791259545772565</v>
+      </c>
+      <c r="L20" s="13">
+        <f t="shared" si="3"/>
+        <v>7.0678915509523925</v>
+      </c>
+      <c r="M20" s="13">
+        <f t="shared" si="3"/>
+        <v>7.2602261422780163</v>
+      </c>
+      <c r="N20" s="13">
+        <f t="shared" si="3"/>
+        <v>7.4454792005567185</v>
+      </c>
+      <c r="O20" s="13">
+        <f t="shared" si="3"/>
+        <v>7.5735285445732092</v>
+      </c>
+      <c r="P20" s="13">
+        <f t="shared" si="3"/>
+        <v>7.6991775489438083</v>
+      </c>
+      <c r="Q20" s="14">
+        <f t="shared" si="3"/>
+        <v>7.7440539607438872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>